<commit_message>
Rounding measurement + adding sensors
</commit_message>
<xml_diff>
--- a/Temperatuur sensoren.xlsx
+++ b/Temperatuur sensoren.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DiskStation\Data\Mijn projecten\Monitoring vloerverwarming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\TemperatureMonitor_MQTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DCF508-8B20-43D8-B7A9-8DA210A78029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47D2BB0-24C5-454F-B7F2-7AA5B224A460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="225" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25575" yWindow="3840" windowWidth="21600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -46,6 +46,51 @@
   </si>
   <si>
     <t>282bfe571f64ff</t>
+  </si>
+  <si>
+    <t>Kring 1 aanvoer</t>
+  </si>
+  <si>
+    <t>Kring 1 afvoer</t>
+  </si>
+  <si>
+    <t>Kring 2 aanvoer</t>
+  </si>
+  <si>
+    <t>Kring 2 afvoer</t>
+  </si>
+  <si>
+    <t>Aanvoer</t>
+  </si>
+  <si>
+    <t>28072261300627</t>
+  </si>
+  <si>
+    <t>280722613294cc</t>
+  </si>
+  <si>
+    <t>280722614c7990</t>
+  </si>
+  <si>
+    <t>280922545d1f8a</t>
+  </si>
+  <si>
+    <t>28092254776424</t>
+  </si>
+  <si>
+    <t>Kring 3 aanvoer</t>
+  </si>
+  <si>
+    <t>Kring 3 afvoer</t>
+  </si>
+  <si>
+    <t>Kring 4 aanvoer</t>
+  </si>
+  <si>
+    <t>Kring 4 afvoer</t>
+  </si>
+  <si>
+    <t>Afvoer</t>
   </si>
 </sst>
 </file>
@@ -89,7 +134,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,6 +153,7 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,8 +169,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1F954CC-0BF3-4ADE-88D1-60C4C83EDF1D}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{C1F954CC-0BF3-4ADE-88D1-60C4C83EDF1D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1F954CC-0BF3-4ADE-88D1-60C4C83EDF1D}" name="Table1" displayName="Table1" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{C1F954CC-0BF3-4ADE-88D1-60C4C83EDF1D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{82BFE69E-4975-4C32-93F9-195E551BAA3F}" name="ID" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{F991BB69-7761-4886-B2D1-963CB6E7864E}" name="Sensor"/>
@@ -396,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,25 +466,80 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>